<commit_message>
Adição de arquivos csv
</commit_message>
<xml_diff>
--- a/modelo_lógico.xlsx
+++ b/modelo_lógico.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="TIPO_USUARIOS" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="94">
   <si>
     <t>TIPO_USUARIO</t>
   </si>
@@ -99,128 +99,227 @@
     <t>RAZAO_SOCIAL</t>
   </si>
   <si>
-    <t>aaa</t>
-  </si>
-  <si>
-    <t>bbb</t>
-  </si>
-  <si>
-    <t>ccc</t>
-  </si>
-  <si>
-    <t>ddd</t>
-  </si>
-  <si>
-    <t>eee</t>
-  </si>
-  <si>
-    <t>fff</t>
-  </si>
-  <si>
-    <t>ggg</t>
-  </si>
-  <si>
-    <t>hhh</t>
-  </si>
-  <si>
-    <t>iii</t>
-  </si>
-  <si>
-    <t>jjj</t>
-  </si>
-  <si>
-    <t>kkk</t>
-  </si>
-  <si>
-    <t>lll</t>
-  </si>
-  <si>
-    <t>mmm</t>
-  </si>
-  <si>
-    <t>nnn</t>
-  </si>
-  <si>
-    <t>ooo</t>
-  </si>
-  <si>
-    <t>pp/pp/pppp</t>
-  </si>
-  <si>
-    <t>qq/qq/qqq</t>
-  </si>
-  <si>
-    <t>rr/rr/rrrr</t>
-  </si>
-  <si>
-    <t>ssssssss</t>
-  </si>
-  <si>
-    <t>tttttttt</t>
-  </si>
-  <si>
-    <t>uuuuuuuu</t>
-  </si>
-  <si>
-    <t>vvvvvvvvvv</t>
-  </si>
-  <si>
-    <t>wwwwwwwww</t>
-  </si>
-  <si>
-    <t>xxxxxxxxx</t>
-  </si>
-  <si>
-    <t>yyyyyyyyyyy</t>
-  </si>
-  <si>
-    <t>zzzzzzzzzzz</t>
-  </si>
-  <si>
-    <t>aaaaaaaaaa</t>
-  </si>
-  <si>
-    <t>ppp</t>
-  </si>
-  <si>
-    <t>qqq</t>
-  </si>
-  <si>
-    <t>rrr</t>
-  </si>
-  <si>
-    <t>sss</t>
-  </si>
-  <si>
-    <t>ttt</t>
-  </si>
-  <si>
-    <t>uuu</t>
-  </si>
-  <si>
-    <t>vvv</t>
-  </si>
-  <si>
-    <t>www</t>
-  </si>
-  <si>
-    <t>xxx</t>
-  </si>
-  <si>
-    <t>yyy</t>
-  </si>
-  <si>
-    <t>zzz</t>
-  </si>
-  <si>
     <t>ID_TIPO_SITUACAO</t>
+  </si>
+  <si>
+    <t>Acupuntura</t>
+  </si>
+  <si>
+    <t>Anestesiologia</t>
+  </si>
+  <si>
+    <t>Angiologia</t>
+  </si>
+  <si>
+    <t>Cardiologia</t>
+  </si>
+  <si>
+    <t>Cirurgia Cardiovascular</t>
+  </si>
+  <si>
+    <t>Cirurgia da Mão</t>
+  </si>
+  <si>
+    <t>Cirurgia do Aparelho Digestivo</t>
+  </si>
+  <si>
+    <t>Cirurgia Geral</t>
+  </si>
+  <si>
+    <t>Cirurgia Pediátrica</t>
+  </si>
+  <si>
+    <t>Cirurgia Plástica</t>
+  </si>
+  <si>
+    <t>Cirurgia Torácica</t>
+  </si>
+  <si>
+    <t>Cirurgia Vascular</t>
+  </si>
+  <si>
+    <t>Dermatologia</t>
+  </si>
+  <si>
+    <t>Radioterapia</t>
+  </si>
+  <si>
+    <t>Urologia</t>
+  </si>
+  <si>
+    <t>Pediatria</t>
+  </si>
+  <si>
+    <t>Psiquiatria</t>
+  </si>
+  <si>
+    <t>Agendada</t>
+  </si>
+  <si>
+    <t>Realizada</t>
+  </si>
+  <si>
+    <t>Cancelada</t>
+  </si>
+  <si>
+    <t>SP Medical Group</t>
+  </si>
+  <si>
+    <t>Av. Barão Limeira, 532, São Paulo, SP</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>Admin</t>
+  </si>
+  <si>
+    <t>Médico</t>
+  </si>
+  <si>
+    <t>Paciente</t>
+  </si>
+  <si>
+    <t>Ligia</t>
+  </si>
+  <si>
+    <t>Alexandre</t>
+  </si>
+  <si>
+    <t>Fernando</t>
+  </si>
+  <si>
+    <t>Henrique</t>
+  </si>
+  <si>
+    <t>João</t>
+  </si>
+  <si>
+    <t>Bruno</t>
+  </si>
+  <si>
+    <t>Mariana</t>
+  </si>
+  <si>
+    <t>ligia@gmail.com</t>
+  </si>
+  <si>
+    <t>alexandre@gmail.com</t>
+  </si>
+  <si>
+    <t>fernando@gmail.com</t>
+  </si>
+  <si>
+    <t>henrique@gmail.com</t>
+  </si>
+  <si>
+    <t>joao@hotmail.com</t>
+  </si>
+  <si>
+    <t>bruno@gmail.com</t>
+  </si>
+  <si>
+    <t>mariana@outlook.com</t>
+  </si>
+  <si>
+    <t>Ricardo Lemos</t>
+  </si>
+  <si>
+    <t>Roberto Possarle</t>
+  </si>
+  <si>
+    <t>Helena Strada</t>
+  </si>
+  <si>
+    <t>ricardo.lemos@spmedicalgroup.com.br</t>
+  </si>
+  <si>
+    <t>roberto.possarle@spmedicalgroup.com.br</t>
+  </si>
+  <si>
+    <t>helena.souza@spmedicalgroup.com.br</t>
+  </si>
+  <si>
+    <t>11 3456-7654</t>
+  </si>
+  <si>
+    <t>11 98765-6543</t>
+  </si>
+  <si>
+    <t>11 97208-4453</t>
+  </si>
+  <si>
+    <t>11 3456-6543</t>
+  </si>
+  <si>
+    <t>11 7656-6377</t>
+  </si>
+  <si>
+    <t>11 95436-8769</t>
+  </si>
+  <si>
+    <t>43522543-5</t>
+  </si>
+  <si>
+    <t>32654345-7</t>
+  </si>
+  <si>
+    <t>54636525-3</t>
+  </si>
+  <si>
+    <t>54366362-5</t>
+  </si>
+  <si>
+    <t>54566266-7</t>
+  </si>
+  <si>
+    <t>54566266-8</t>
+  </si>
+  <si>
+    <t>Rua Estado de Israel 240, São Paulo, Estado de São Paulo, 04022-000</t>
+  </si>
+  <si>
+    <t>Av. Paulista, 1578 - Bela Vista, São Paulo - SP, 01310-200</t>
+  </si>
+  <si>
+    <t>Av. Ibirapuera - Indianópolis, 2927,  São Paulo - SP, 04029-200</t>
+  </si>
+  <si>
+    <t>R. Vitória, 120 - Vila Sao Jorge, Barueri - SP, 06402-030</t>
+  </si>
+  <si>
+    <t>R. Ver. Geraldo de Camargo, 66 - Santa Luzia, Ribeirão Pires - SP, 09405-380</t>
+  </si>
+  <si>
+    <t>Alameda dos Arapanés, 945 - Indianópolis, São Paulo - SP, 04524-001</t>
+  </si>
+  <si>
+    <t>R Sao Antonio, 232 - Vila Universal, Barueri - SP, 06407-140</t>
+  </si>
+  <si>
+    <t>32544444-1</t>
+  </si>
+  <si>
+    <t>54356-SP</t>
+  </si>
+  <si>
+    <t>53452-SP</t>
+  </si>
+  <si>
+    <t>65463-SP</t>
+  </si>
+  <si>
+    <t>admin@admin.com</t>
+  </si>
+  <si>
+    <t>Administrador</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,14 +330,6 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -291,7 +382,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -299,7 +390,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -580,10 +674,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -592,25 +686,28 @@
     <col min="2" max="2" width="8.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>24</v>
-      </c>
+        <v>48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E11" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -620,18 +717,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.21875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="6.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="36.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -650,67 +748,199 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>93</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>49</v>
+      </c>
+      <c r="B3" s="2">
+        <v>3</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>32</v>
+        <v>56</v>
+      </c>
+      <c r="D3" s="2">
+        <v>123456</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>24</v>
+        <v>50</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>33</v>
+        <v>57</v>
+      </c>
+      <c r="D4" s="2">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="2">
+        <v>3</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" s="2">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" s="2">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D6" s="2">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D7" s="2">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="2">
+        <v>3</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D8" s="2">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="2">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="2">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="2">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="2">
+        <v>2</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="2">
+        <v>123456</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B12" s="2">
+        <v>2</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="2">
+        <v>123456</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" r:id="rId1" display="ligia@gmail.com"/>
+    <hyperlink ref="B4" r:id="rId2" display="alexandre@gmail.com"/>
+    <hyperlink ref="B5" r:id="rId3" display="fernando@gmail.com"/>
+    <hyperlink ref="B6" r:id="rId4" display="henrique@gmail.com"/>
+    <hyperlink ref="B7" r:id="rId5" display="joao@hotmail.com"/>
+    <hyperlink ref="B8" r:id="rId6" display="bruno@gmail.com"/>
+    <hyperlink ref="B9" r:id="rId7" display="mariana@outlook.com"/>
+    <hyperlink ref="C3" r:id="rId8"/>
+    <hyperlink ref="C4" r:id="rId9"/>
+    <hyperlink ref="C5" r:id="rId10"/>
+    <hyperlink ref="C6" r:id="rId11"/>
+    <hyperlink ref="C7" r:id="rId12"/>
+    <hyperlink ref="C8" r:id="rId13"/>
+    <hyperlink ref="C9" r:id="rId14"/>
+    <hyperlink ref="C10" r:id="rId15"/>
+    <hyperlink ref="C11" r:id="rId16"/>
+    <hyperlink ref="C12" r:id="rId17"/>
+    <hyperlink ref="C2" r:id="rId18"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="66.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
@@ -734,63 +964,141 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>37</v>
+      <c r="A2" s="2">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2">
+        <v>30602</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>40</v>
+        <v>69</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>46</v>
+        <v>75</v>
+      </c>
+      <c r="E2" s="2">
+        <v>94839859000</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>23</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>38</v>
+      <c r="A3" s="2">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2">
+        <v>37095</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>41</v>
+        <v>70</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>47</v>
+        <v>76</v>
+      </c>
+      <c r="E3" s="2">
+        <v>73556944057</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>24</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>39</v>
+      <c r="A4" s="2">
+        <v>4</v>
+      </c>
+      <c r="B4" s="2">
+        <v>28773</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>48</v>
+        <v>77</v>
+      </c>
+      <c r="E4" s="2">
+        <v>16839338002</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>25</v>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>5</v>
+      </c>
+      <c r="B5" s="2">
+        <v>31333</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="2">
+        <v>14332654765</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>6</v>
+      </c>
+      <c r="B6" s="2">
+        <v>27633</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="2">
+        <v>91305348010</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>26379</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7" s="2">
+        <v>79799299004</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2">
+        <v>43164</v>
+      </c>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="2">
+        <v>13771913039</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -800,10 +1108,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="A9" sqref="A9:T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -815,7 +1123,7 @@
     <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -829,59 +1137,112 @@
         <v>14</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>51</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" s="2">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2">
+        <v>43485.625</v>
+      </c>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2">
+        <v>43106.416666666664</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>10</v>
+      </c>
+      <c r="C4" s="2">
+        <v>43503.458333333336</v>
+      </c>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
+        <v>10</v>
+      </c>
+      <c r="C5" s="2">
+        <v>43137.416666666664</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2">
+        <v>43503.458854166667</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2">
+        <v>43504.625</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2">
+        <v>43505.458854166667</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -895,10 +1256,13 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -907,17 +1271,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>22</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -930,13 +1294,13 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
@@ -961,53 +1325,53 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>26</v>
+        <v>63</v>
+      </c>
+      <c r="C2" s="2">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>53</v>
+        <v>90</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>27</v>
+        <v>64</v>
+      </c>
+      <c r="C3" s="2">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>54</v>
+        <v>91</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>28</v>
+        <v>65</v>
+      </c>
+      <c r="C4" s="2">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2">
+        <v>16</v>
+      </c>
+      <c r="E4" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -1017,15 +1381,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:A18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -1035,17 +1399,87 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2" t="s">
         <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1055,16 +1489,17 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
@@ -1079,39 +1514,18 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
-        <v>32</v>
+      <c r="A2" s="4">
+        <v>86400902000130</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>